<commit_message>
Adicionando novos arquivos da aula de backend
</commit_message>
<xml_diff>
--- a/Banco de dados/Modelagem Banco de Dados/Aula 06/excel/Aula 06 - Feito em aula.xlsx
+++ b/Banco de dados/Modelagem Banco de Dados/Aula 06/excel/Aula 06 - Feito em aula.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\Documents\GitHub\aulas-graduacao\Banco de dados\Modelagem Banco de Dados\Aula 06\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9322B67-D086-45A5-93FC-91AF7C006D5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43C009E-BB4C-4DE7-80BE-F9E9942D51B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18570" yWindow="1125" windowWidth="17715" windowHeight="14010" activeTab="3" xr2:uid="{10A57BE7-EA12-45C1-BA0B-768593439AAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="9" activeTab="15" xr2:uid="{10A57BE7-EA12-45C1-BA0B-768593439AAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades fortes" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="166">
   <si>
     <t>Funcionario</t>
   </si>
@@ -445,6 +445,108 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>ID_Func</t>
+  </si>
+  <si>
+    <t>Funcionário</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Santa Catarina</t>
+  </si>
+  <si>
+    <t>Bahia</t>
+  </si>
+  <si>
+    <t>Amazonas</t>
+  </si>
+  <si>
+    <t>Campinas</t>
+  </si>
+  <si>
+    <t>Paraty</t>
+  </si>
+  <si>
+    <t>Blumenau</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t>Manaus</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>EUA</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Dependência Funcional</t>
+  </si>
+  <si>
+    <t>Transitividade</t>
+  </si>
+  <si>
+    <t>Dependência Funcional irredutivel à esquerda</t>
+  </si>
+  <si>
+    <t>Dependência multivalorada</t>
+  </si>
+  <si>
+    <t>Dependentes</t>
+  </si>
+  <si>
+    <t>Fabiana</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>SIGLA</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>SELECT * FROM TABELA</t>
+  </si>
+  <si>
+    <t>CLASS A {}</t>
   </si>
 </sst>
 </file>
@@ -454,7 +556,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,8 +627,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,8 +674,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -690,12 +819,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -717,25 +866,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -751,6 +885,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -759,33 +919,6 @@
   <dxfs count="76">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -802,14 +935,14 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -819,10 +952,37 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1676,7 +1836,7 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A6BA1DE6-BA01-43AA-84A4-2C17B1F24A5E}" name="Tabela216205" displayName="Tabela216205" ref="J7:M9" totalsRowShown="0" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A6BA1DE6-BA01-43AA-84A4-2C17B1F24A5E}" name="Tabela216205" displayName="Tabela216205" ref="J7:M9" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="J7:M9" xr:uid="{6A473787-6F9E-4594-87A3-5AEE6F4F11F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1696,7 +1856,7 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{BFC93B33-4960-4EBA-9302-0DAAB9D04D4C}" name="Tabela21620526" displayName="Tabela21620526" ref="J26:M28" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{BFC93B33-4960-4EBA-9302-0DAAB9D04D4C}" name="Tabela21620526" displayName="Tabela21620526" ref="J26:M28" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="J26:M28" xr:uid="{7C3EC5A0-54C9-4695-B785-9837CABBA18F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1706,7 +1866,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D9FB0626-BA34-4B7C-BBA5-88830DBD81E2}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{3A783258-A418-4611-9318-58A118023746}" name="Nome"/>
-    <tableColumn id="4" xr3:uid="{4D5F0072-2C5A-4B93-9CC4-069672B2D2DD}" name="ID_Funcionario" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{4D5F0072-2C5A-4B93-9CC4-069672B2D2DD}" name="ID_Funcionario" dataDxfId="6">
       <calculatedColumnFormula>2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{2A895D39-F263-4F0E-952B-B6996D6F6430}" name="DataInicio"/>
@@ -1716,13 +1876,13 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{7EB2A8F0-B6CB-443A-99DB-2BC73A637E97}" name="Tabela51822242527" displayName="Tabela51822242527" ref="J33:K38" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{7EB2A8F0-B6CB-443A-99DB-2BC73A637E97}" name="Tabela51822242527" displayName="Tabela51822242527" ref="J33:K38" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="J33:K38" xr:uid="{16135503-FBE0-427B-8B87-1B49C54D784C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{98112E11-6E9F-4BBA-B8B0-077FD1ED2A6C}" name="Numero_Dept" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{98112E11-6E9F-4BBA-B8B0-077FD1ED2A6C}" name="Numero_Dept" dataDxfId="3">
       <calculatedColumnFormula>D25</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{F1661DCB-7BBA-41AE-823E-AA434F0D9D22}" name="Local"/>
@@ -1732,7 +1892,7 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{29EB37E5-81A1-4109-8739-87C8EB37DE9A}" name="Tabela21620528" displayName="Tabela21620528" ref="C15:F17" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{29EB37E5-81A1-4109-8739-87C8EB37DE9A}" name="Tabela21620528" displayName="Tabela21620528" ref="C15:F17" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="C15:F17" xr:uid="{6A473787-6F9E-4594-87A3-5AEE6F4F11F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1742,7 +1902,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C74541C7-A7EC-4F64-B659-A090F654374D}" name="Numero"/>
     <tableColumn id="2" xr3:uid="{F2EB8281-A5AB-49CD-AB4D-8B7BD0028F8F}" name="Nome"/>
-    <tableColumn id="4" xr3:uid="{6CA63538-DF7B-4492-A447-97386903EFC1}" name="ID_Funcionario" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{6CA63538-DF7B-4492-A447-97386903EFC1}" name="ID_Funcionario" dataDxfId="0">
       <calculatedColumnFormula>Tabela11519[[#This Row],[ID]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F5D986E3-AAE5-4815-B817-382D7538F240}" name="DataInicio"/>
@@ -2275,8 +2435,8 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,66 +2444,67 @@
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="A2" s="26"/>
+      <c r="Q2" s="26"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="Q3" s="31"/>
+      <c r="A3" s="26"/>
+      <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="Q4" s="31"/>
+      <c r="A4" s="26"/>
+      <c r="Q4" s="26"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="Q5" s="31"/>
+      <c r="A5" s="26"/>
+      <c r="Q5" s="26"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="Q6" s="31"/>
+      <c r="A6" s="26"/>
+      <c r="Q6" s="26"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="C7" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="30" t="s">
+      <c r="A7" s="26"/>
+      <c r="C7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="25" t="s">
         <v>124</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -2358,10 +2519,10 @@
       <c r="M7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="31"/>
+      <c r="Q7" s="26"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="26"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
@@ -2395,10 +2556,10 @@
       <c r="M8" s="9">
         <v>43490</v>
       </c>
-      <c r="Q8" s="31"/>
+      <c r="Q8" s="26"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="26"/>
       <c r="C9" s="4">
         <v>2</v>
       </c>
@@ -2432,10 +2593,10 @@
       <c r="M9" s="9">
         <v>42287</v>
       </c>
-      <c r="Q9" s="31"/>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="26"/>
       <c r="C10" s="4">
         <v>3</v>
       </c>
@@ -2456,10 +2617,10 @@
         <f>VLOOKUP(G10,Tabela216205[#All],2,FALSE)</f>
         <v>RH</v>
       </c>
-      <c r="Q10" s="31"/>
+      <c r="Q10" s="26"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="26"/>
       <c r="C11" s="4">
         <v>4</v>
       </c>
@@ -2480,10 +2641,10 @@
         <f>VLOOKUP(G11,Tabela216205[#All],2,FALSE)</f>
         <v>TI</v>
       </c>
-      <c r="Q11" s="31"/>
+      <c r="Q11" s="26"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="26"/>
       <c r="C12" s="4">
         <v>5</v>
       </c>
@@ -2504,90 +2665,90 @@
         <f>VLOOKUP(G12,Tabela216205[#All],2,FALSE)</f>
         <v>TI</v>
       </c>
-      <c r="Q12" s="31"/>
+      <c r="Q12" s="26"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="Q13" s="31"/>
+      <c r="A13" s="26"/>
+      <c r="Q13" s="26"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="Q14" s="31"/>
+      <c r="A14" s="26"/>
+      <c r="Q14" s="26"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="Q15" s="31"/>
+      <c r="A15" s="26"/>
+      <c r="Q15" s="26"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="Q16" s="31"/>
+      <c r="A16" s="26"/>
+      <c r="Q16" s="26"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="Q17" s="31"/>
+      <c r="A17" s="26"/>
+      <c r="Q17" s="26"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="Q18" s="31"/>
+      <c r="A18" s="26"/>
+      <c r="Q18" s="26"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="Q19" s="31"/>
+      <c r="A19" s="26"/>
+      <c r="Q19" s="26"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="Q20" s="31"/>
+      <c r="A20" s="26"/>
+      <c r="Q20" s="26"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="Q21" s="31"/>
+      <c r="A21" s="26"/>
+      <c r="Q21" s="26"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="Q22" s="31"/>
+      <c r="A22" s="26"/>
+      <c r="Q22" s="26"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="Q24" s="31"/>
+      <c r="A24" s="26"/>
+      <c r="Q24" s="26"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="Q25" s="31"/>
+      <c r="A25" s="26"/>
+      <c r="Q25" s="26"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="C26" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="30" t="s">
+      <c r="A26" s="26"/>
+      <c r="C26" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="30" t="s">
+      <c r="G26" s="25" t="s">
         <v>10</v>
       </c>
       <c r="J26" s="5" t="s">
@@ -2602,10 +2763,10 @@
       <c r="M26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Q26" s="31"/>
+      <c r="Q26" s="26"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="26"/>
       <c r="C27" s="4">
         <v>1</v>
       </c>
@@ -2635,10 +2796,10 @@
       <c r="M27" s="9">
         <v>43490</v>
       </c>
-      <c r="Q27" s="31"/>
+      <c r="Q27" s="26"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="26"/>
       <c r="C28" s="4">
         <v>2</v>
       </c>
@@ -2668,10 +2829,10 @@
       <c r="M28" s="9">
         <v>42287</v>
       </c>
-      <c r="Q28" s="31"/>
+      <c r="Q28" s="26"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="26"/>
       <c r="C29" s="4">
         <v>3</v>
       </c>
@@ -2688,10 +2849,10 @@
         <f>J28</f>
         <v>2</v>
       </c>
-      <c r="Q29" s="31"/>
+      <c r="Q29" s="26"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="26"/>
       <c r="C30" s="4">
         <v>4</v>
       </c>
@@ -2708,10 +2869,10 @@
         <f>J27</f>
         <v>1</v>
       </c>
-      <c r="Q30" s="31"/>
+      <c r="Q30" s="26"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="26"/>
       <c r="C31" s="4">
         <v>5</v>
       </c>
@@ -2728,24 +2889,24 @@
         <f>J27</f>
         <v>1</v>
       </c>
-      <c r="Q31" s="31"/>
+      <c r="Q31" s="26"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="Q32" s="31"/>
+      <c r="A32" s="26"/>
+      <c r="Q32" s="26"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="A33" s="26"/>
       <c r="J33" s="5" t="s">
         <v>41</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="Q33" s="31"/>
+      <c r="Q33" s="26"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="A34" s="26"/>
       <c r="J34">
         <f>$J$8</f>
         <v>1</v>
@@ -2753,10 +2914,10 @@
       <c r="K34" t="s">
         <v>43</v>
       </c>
-      <c r="Q34" s="31"/>
+      <c r="Q34" s="26"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+      <c r="A35" s="26"/>
       <c r="J35">
         <f t="shared" ref="J35:J37" si="0">$J$8</f>
         <v>1</v>
@@ -2764,10 +2925,10 @@
       <c r="K35" t="s">
         <v>44</v>
       </c>
-      <c r="Q35" s="31"/>
+      <c r="Q35" s="26"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+      <c r="A36" s="26"/>
       <c r="J36">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2775,10 +2936,10 @@
       <c r="K36" t="s">
         <v>45</v>
       </c>
-      <c r="Q36" s="31"/>
+      <c r="Q36" s="26"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
+      <c r="A37" s="26"/>
       <c r="J37">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2786,44 +2947,44 @@
       <c r="K37" t="s">
         <v>46</v>
       </c>
-      <c r="Q37" s="31"/>
+      <c r="Q37" s="26"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
+      <c r="A38" s="26"/>
       <c r="J38" s="12">
         <v>2</v>
       </c>
       <c r="K38" t="s">
         <v>43</v>
       </c>
-      <c r="Q38" s="31"/>
+      <c r="Q38" s="26"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="Q39" s="31"/>
+      <c r="A39" s="26"/>
+      <c r="Q39" s="26"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="Q40" s="31"/>
+      <c r="A40" s="26"/>
+      <c r="Q40" s="26"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2843,8 +3004,8 @@
   </sheetPr>
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,65 +3020,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="A2" s="26"/>
+      <c r="Q2" s="26"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="Q3" s="31"/>
+      <c r="A3" s="26"/>
+      <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="Q4" s="31"/>
+      <c r="A4" s="26"/>
+      <c r="Q4" s="26"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="Q5" s="31"/>
+      <c r="A5" s="26"/>
+      <c r="Q5" s="26"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="Q6" s="31"/>
+      <c r="A6" s="26"/>
+      <c r="Q6" s="26"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="C7" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="30" t="s">
+      <c r="A7" s="26"/>
+      <c r="C7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="31"/>
+      <c r="Q7" s="26"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="26"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
@@ -2927,16 +3088,16 @@
       <c r="E8" s="4">
         <v>132465789</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="22">
         <v>4200</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
       </c>
-      <c r="Q8" s="31"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="Q8" s="26"/>
+    </row>
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
       <c r="C9" s="4">
         <v>2</v>
       </c>
@@ -2946,16 +3107,16 @@
       <c r="E9" s="4">
         <v>132465798</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="22">
         <v>5000</v>
       </c>
       <c r="G9" s="4">
         <v>2</v>
       </c>
-      <c r="Q9" s="31"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="Q9" s="26"/>
+    </row>
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
       <c r="C10" s="4">
         <v>3</v>
       </c>
@@ -2965,17 +3126,17 @@
       <c r="E10" s="4">
         <v>69587485</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="22">
         <v>12000</v>
       </c>
       <c r="G10" s="4">
         <f>C17</f>
         <v>2</v>
       </c>
-      <c r="Q10" s="31"/>
+      <c r="Q10" s="26"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="26"/>
       <c r="C11" s="4">
         <v>4</v>
       </c>
@@ -2985,17 +3146,17 @@
       <c r="E11" s="4">
         <v>123465798</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="22">
         <v>6000</v>
       </c>
       <c r="G11" s="4">
         <f>C16</f>
         <v>1</v>
       </c>
-      <c r="Q11" s="31"/>
+      <c r="Q11" s="26"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="26"/>
       <c r="C12" s="4">
         <v>5</v>
       </c>
@@ -3005,25 +3166,25 @@
       <c r="E12" s="4">
         <v>55566688</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="22">
         <v>12000</v>
       </c>
       <c r="G12" s="4">
         <f>C16</f>
         <v>1</v>
       </c>
-      <c r="Q12" s="31"/>
+      <c r="Q12" s="26"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="Q13" s="31"/>
+      <c r="A13" s="26"/>
+      <c r="Q13" s="26"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="Q14" s="31"/>
+      <c r="A14" s="26"/>
+      <c r="Q14" s="26"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="26"/>
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
@@ -3036,10 +3197,10 @@
       <c r="F15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Q15" s="31"/>
+      <c r="Q15" s="26"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="26"/>
       <c r="C16">
         <v>1</v>
       </c>
@@ -3052,10 +3213,10 @@
       <c r="F16" s="9">
         <v>43490</v>
       </c>
-      <c r="Q16" s="31"/>
+      <c r="Q16" s="26"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="26"/>
       <c r="C17">
         <v>2</v>
       </c>
@@ -3068,79 +3229,79 @@
       <c r="F17" s="9">
         <v>42287</v>
       </c>
-      <c r="Q17" s="31"/>
+      <c r="Q17" s="26"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="26"/>
       <c r="J18" s="12"/>
-      <c r="Q18" s="31"/>
+      <c r="Q18" s="26"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="Q19" s="31"/>
+      <c r="A19" s="26"/>
+      <c r="Q19" s="26"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="Q20" s="31"/>
+      <c r="A20" s="26"/>
+      <c r="Q20" s="26"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="Q21" s="31"/>
+      <c r="A21" s="26"/>
+      <c r="Q21" s="26"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="Q23" s="31"/>
+      <c r="A23" s="26"/>
+      <c r="Q23" s="26"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="Q24" s="31"/>
+      <c r="A24" s="26"/>
+      <c r="Q24" s="26"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="C25" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="30" t="s">
+      <c r="A25" s="26"/>
+      <c r="C25" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25" s="34" t="s">
+      <c r="H25" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="Q25" s="31"/>
+      <c r="Q25" s="26"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="26"/>
       <c r="C26" s="4">
         <v>1</v>
       </c>
@@ -3156,17 +3317,17 @@
       <c r="G26" s="4">
         <v>1</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="30">
         <f>$E$26</f>
         <v>132465789</v>
       </c>
-      <c r="Q26" s="31"/>
+      <c r="Q26" s="26"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="26"/>
       <c r="C27" s="4">
         <v>2</v>
       </c>
@@ -3182,17 +3343,17 @@
       <c r="G27" s="4">
         <v>2</v>
       </c>
-      <c r="H27" s="35" t="s">
+      <c r="H27" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I27" s="30">
         <f>$E$27</f>
         <v>132465798</v>
       </c>
-      <c r="Q27" s="31"/>
+      <c r="Q27" s="26"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="26"/>
       <c r="C28" s="4">
         <v>3</v>
       </c>
@@ -3208,17 +3369,17 @@
       <c r="G28" s="4">
         <v>1</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I28" s="30">
         <f>$E$26</f>
         <v>132465789</v>
       </c>
-      <c r="Q28" s="31"/>
+      <c r="Q28" s="26"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="26"/>
       <c r="C29" s="4">
         <v>4</v>
       </c>
@@ -3234,17 +3395,17 @@
       <c r="G29" s="4">
         <v>1</v>
       </c>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I29" s="30">
         <f>$E$26</f>
         <v>132465789</v>
       </c>
-      <c r="Q29" s="31"/>
+      <c r="Q29" s="26"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="26"/>
       <c r="C30" s="4">
         <v>5</v>
       </c>
@@ -3260,69 +3421,69 @@
       <c r="G30" s="4">
         <v>2</v>
       </c>
-      <c r="H30" s="35" t="s">
+      <c r="H30" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="35">
+      <c r="I30" s="30">
         <f>$E$27</f>
         <v>132465798</v>
       </c>
-      <c r="Q30" s="31"/>
+      <c r="Q30" s="26"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="Q31" s="31"/>
+      <c r="A31" s="26"/>
+      <c r="Q31" s="26"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="Q32" s="31"/>
+      <c r="A32" s="26"/>
+      <c r="Q32" s="26"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="Q33" s="31"/>
+      <c r="A33" s="26"/>
+      <c r="Q33" s="26"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="Q34" s="31"/>
+      <c r="A34" s="26"/>
+      <c r="Q34" s="26"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="Q35" s="31"/>
+      <c r="A35" s="26"/>
+      <c r="Q35" s="26"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="Q36" s="31"/>
+      <c r="A36" s="26"/>
+      <c r="Q36" s="26"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="Q37" s="31"/>
+      <c r="A37" s="26"/>
+      <c r="Q37" s="26"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="Q38" s="31"/>
+      <c r="A38" s="26"/>
+      <c r="Q38" s="26"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="Q39" s="31"/>
+      <c r="A39" s="26"/>
+      <c r="Q39" s="26"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-      <c r="Q40" s="31"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3353,25 +3514,25 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="34" t="s">
+      <c r="G3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="29" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3391,10 +3552,10 @@
       <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="30">
         <v>1</v>
       </c>
     </row>
@@ -3414,10 +3575,10 @@
       <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="30">
         <v>2</v>
       </c>
     </row>
@@ -3437,10 +3598,10 @@
       <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="30">
         <v>1</v>
       </c>
     </row>
@@ -3460,10 +3621,10 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="30">
         <v>1</v>
       </c>
     </row>
@@ -3483,10 +3644,10 @@
       <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="30">
         <v>2</v>
       </c>
     </row>
@@ -3565,25 +3726,25 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="34" t="s">
+      <c r="G3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="29" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3603,10 +3764,10 @@
       <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="30">
         <v>1</v>
       </c>
     </row>
@@ -3626,10 +3787,10 @@
       <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="30">
         <v>2</v>
       </c>
     </row>
@@ -3649,10 +3810,10 @@
       <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="30">
         <v>1</v>
       </c>
     </row>
@@ -3672,10 +3833,10 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="30">
         <v>1</v>
       </c>
     </row>
@@ -3695,37 +3856,37 @@
       <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32">
         <v>6</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="32">
         <v>556677889</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="32">
         <v>5000</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="32">
         <v>3</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="32">
         <v>3</v>
       </c>
-      <c r="I9" s="36"/>
+      <c r="I9" s="31"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -3779,25 +3940,25 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="27" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3922,30 +4083,30 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34">
         <v>6</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="34">
         <v>556677889</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="34">
         <v>5000</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="34">
         <v>3</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9" s="35">
         <f>B9</f>
         <v>6</v>
       </c>
-      <c r="I9" s="38"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -3986,8 +4147,8 @@
   </sheetPr>
   <dimension ref="A3:F61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3998,16 +4159,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="28" t="s">
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="27" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4082,29 +4243,36 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34">
         <v>6</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="38"/>
+      <c r="F9" s="33"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="28" t="s">
+      <c r="B50" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="23" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4164,21 +4332,21 @@
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="39">
+      <c r="B56" s="34">
         <v>6</v>
       </c>
-      <c r="C56" s="39" t="s">
+      <c r="C56" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="35" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="41" t="s">
+      <c r="B59" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="36" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4199,33 +4367,45 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B49:D49"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A28D41-069E-4530-BE72-E57E92B4D8CC}">
-  <dimension ref="C4:H10"/>
+  <dimension ref="B2:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B43" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+    </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
@@ -4254,14 +4434,18 @@
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="21">
         <v>132465789</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="22">
         <v>4200</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -4270,14 +4454,18 @@
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="21">
         <v>132465798</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="22">
         <v>5000</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -4286,14 +4474,18 @@
       <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="21">
         <v>69587485</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="22">
         <v>12000</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -4302,14 +4494,18 @@
       <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="21">
         <v>123465798</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="22">
         <v>6000</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="G9" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -4318,20 +4514,444 @@
       <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="21">
         <v>55566688</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="22">
         <v>12000</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="G10" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" s="51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="21">
+        <v>132465789</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" s="21">
+        <v>132465789</v>
+      </c>
+      <c r="I44" s="48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="21">
+        <v>132465798</v>
+      </c>
+      <c r="F45" s="2">
+        <v>2</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" s="21">
+        <v>132465798</v>
+      </c>
+      <c r="I45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="21">
+        <v>69587485</v>
+      </c>
+      <c r="F46" s="2">
+        <v>3</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" s="21">
+        <v>69587485</v>
+      </c>
+      <c r="I46" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>4</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="21">
+        <v>123465798</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H47" s="21">
+        <v>123465798</v>
+      </c>
+      <c r="I47" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="21">
+        <v>55566688</v>
+      </c>
+      <c r="F48" s="2">
+        <v>5</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H48" s="21">
+        <v>55566688</v>
+      </c>
+      <c r="I48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>161</v>
+      </c>
+      <c r="H51" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f>B44</f>
+        <v>1</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>163</v>
+      </c>
+      <c r="H52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f>B44</f>
+        <v>1</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f>B44</f>
+        <v>1</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f>B47</f>
+        <v>4</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="2">
+        <f>B48</f>
+        <v>5</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="2">
+        <f>B47</f>
+        <v>4</v>
+      </c>
+      <c r="D57" s="47" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:H4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4461,17 +5081,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="I1" s="19" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="I1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -4543,17 +5163,17 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="I8" s="19" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="I8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -4650,7 +5270,7 @@
   </sheetPr>
   <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -4665,19 +5285,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="G1" s="21" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="G1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -4783,17 +5403,17 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="G8" s="19" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="G8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -4906,21 +5526,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
       <c r="G1" s="10"/>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -5058,18 +5678,18 @@
       <c r="G6" s="12"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="I8" s="19" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="I8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -5193,21 +5813,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
       <c r="G1" s="10"/>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -5387,18 +6007,18 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="I9" s="19" t="s">
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="I9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -5524,21 +6144,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
       <c r="G2" s="10"/>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
@@ -5717,8 +6337,8 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -5742,18 +6362,18 @@
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="I12" s="19" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="I12" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
@@ -5838,16 +6458,16 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="15"/>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="J19" s="20"/>
+      <c r="J19" s="39"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
@@ -6642,13 +7262,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="19" t="s">
         <v>73</v>
       </c>
     </row>
@@ -6675,10 +7295,10 @@
       <c r="D4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="19" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>